<commit_message>
+ show entries datatables & perbaikan impor periode & penamaan file export
</commit_message>
<xml_diff>
--- a/public/template/Template Import User Alumni.xlsx
+++ b/public/template/Template Import User Alumni.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\tracer\storage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\tracer\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625FEA83-293F-48C5-BF1E-1D75683E5074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C46C2D9-A35E-4C03-8D26-DB3231CA699C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{25E3BB40-640E-44D8-A8BB-0A45A82EC1AB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{25E3BB40-640E-44D8-A8BB-0A45A82EC1AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -536,7 +536,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>2022/2024 Genap</t>
+      <t>2022/2024</t>
     </r>
     <r>
       <rPr>
@@ -551,7 +551,7 @@
     </r>
   </si>
   <si>
-    <t>2022/2023 Genap</t>
+    <t>2024/2025</t>
   </si>
 </sst>
 </file>
@@ -683,7 +683,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -706,7 +706,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1024,17 +1023,17 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1065,20 +1064,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE08366-BDFE-4F3B-A4DB-26D9E60BE20A}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="66.85546875" customWidth="1"/>
+    <col min="1" max="1" width="66.88671875" customWidth="1"/>
     <col min="2" max="2" width="66" customWidth="1"/>
-    <col min="3" max="4" width="65.7109375" customWidth="1"/>
-    <col min="5" max="5" width="62.85546875" customWidth="1"/>
-    <col min="6" max="6" width="64.140625" customWidth="1"/>
+    <col min="3" max="4" width="65.6640625" customWidth="1"/>
+    <col min="5" max="5" width="62.88671875" customWidth="1"/>
+    <col min="6" max="6" width="64.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1098,7 +1097,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1118,7 +1117,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1128,7 +1127,7 @@
       <c r="C3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -1139,7 +1138,7 @@
       </c>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C4" s="6" t="s">
         <v>0</v>
       </c>
@@ -1149,7 +1148,7 @@
       </c>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C5" s="6" t="s">
         <v>7</v>
       </c>
@@ -1159,7 +1158,7 @@
       </c>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C6" s="6" t="s">
         <v>8</v>
       </c>
@@ -1169,62 +1168,62 @@
       </c>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C7" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="6"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C8" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="6"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C9" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="6"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C10" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="6"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C11" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="6"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C12" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="6"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C13" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="1"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H15" s="4"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
- fix mekanisme survey alumni
</commit_message>
<xml_diff>
--- a/public/template/Template Import User Alumni.xlsx
+++ b/public/template/Template Import User Alumni.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\tracer\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C46C2D9-A35E-4C03-8D26-DB3231CA699C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C05912-08BA-4C28-B352-C0E57F7A02C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{25E3BB40-640E-44D8-A8BB-0A45A82EC1AB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{25E3BB40-640E-44D8-A8BB-0A45A82EC1AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>D3 Farmasi</t>
   </si>
@@ -552,6 +552,72 @@
   </si>
   <si>
     <t>2024/2025</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">kolom pertama: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nik</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">pada kolom </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nik</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> hanya diisi menggunakan angka (contoh:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 603034204821001</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -683,7 +749,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -706,6 +772,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1020,36 +1087,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{474205F8-1B75-4B58-A18A-CBD851E01D53}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="10">
+        <v>603034204821001</v>
+      </c>
+      <c r="B1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="D1">
+      <c r="E1">
         <v>2001</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1062,169 +1133,179 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE08366-BDFE-4F3B-A4DB-26D9E60BE20A}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.88671875" customWidth="1"/>
-    <col min="2" max="2" width="66" customWidth="1"/>
-    <col min="3" max="4" width="65.6640625" customWidth="1"/>
-    <col min="5" max="5" width="62.88671875" customWidth="1"/>
-    <col min="6" max="6" width="64.109375" customWidth="1"/>
+    <col min="1" max="1" width="74" customWidth="1"/>
+    <col min="2" max="2" width="66.85546875" customWidth="1"/>
+    <col min="3" max="3" width="66" customWidth="1"/>
+    <col min="4" max="5" width="65.7109375" customWidth="1"/>
+    <col min="6" max="6" width="62.85546875" customWidth="1"/>
+    <col min="7" max="7" width="64.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C4" s="6" t="s">
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="F4" s="6" t="s">
+      <c r="E4" s="6"/>
+      <c r="G4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C5" s="6" t="s">
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="F5" s="6" t="s">
+      <c r="E5" s="6"/>
+      <c r="G5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C6" s="6" t="s">
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="F6" s="1" t="s">
+      <c r="E6" s="6"/>
+      <c r="G6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C7" s="6" t="s">
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C8" s="6" t="s">
+      <c r="E7" s="6"/>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C9" s="6" t="s">
+      <c r="E8" s="6"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C10" s="6" t="s">
+      <c r="E9" s="6"/>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C11" s="6" t="s">
+      <c r="E10" s="6"/>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C12" s="6" t="s">
+      <c r="E11" s="6"/>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C13" s="1" t="s">
+      <c r="E12" s="6"/>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H15" s="4"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
+      <c r="E13" s="1"/>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I15" s="4"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>